<commit_message>
Refactor, and add pydemos.
</commit_message>
<xml_diff>
--- a/apitest/TestCases.xlsx
+++ b/apitest/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengjin/Workspaces/zj_py3_project/interfacetest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengjin/Workspaces/zj_py3_project/apitest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7F48C040-29DC-DA48-A397-7739766CC6D2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6F599F92-0781-4A4B-94C6-5ECC96736E41}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{C6BC2A70-CB81-DB40-9C8F-527C04FB6517}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>CaseId</t>
   </si>
@@ -73,13 +73,19 @@
   </si>
   <si>
     <t>k1=v1&amp;k2=v2</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:17891/index</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -91,6 +97,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,15 +148,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -455,22 +472,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E798D7C-3FAD-754F-9877-91756B700D0C}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="35.1640625" customWidth="1"/>
-    <col min="5" max="5" width="44.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="28" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" customWidth="1"/>
+    <col min="6" max="6" width="44.6640625" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -481,19 +499,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -503,20 +524,23 @@
       <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>200</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -526,20 +550,23 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>200</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -547,8 +574,13 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{EC47FDFA-BB4B-4C4E-9638-E51829180CCB}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{F4D51686-6BC4-144F-B552-4DC7D886A320}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Add load cases fn, and refactor.
</commit_message>
<xml_diff>
--- a/apitest/TestCases.xlsx
+++ b/apitest/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengjin/Workspaces/zj_py3_project/apitest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6F599F92-0781-4A4B-94C6-5ECC96736E41}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{07BAA859-3BE3-D846-B7DD-347099F2B890}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{C6BC2A70-CB81-DB40-9C8F-527C04FB6517}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>CaseId</t>
   </si>
@@ -42,15 +42,6 @@
     <t>Body</t>
   </si>
   <si>
-    <t>ExpectedCode</t>
-  </si>
-  <si>
-    <t>http_get_test_01</t>
-  </si>
-  <si>
-    <t>Content-Type:'text/json; charset=utf-8'</t>
-  </si>
-  <si>
     <t>{"email": "123456@163.com", "password": "123456"}</t>
   </si>
   <si>
@@ -60,18 +51,12 @@
     <t>{"results": "ok"}</t>
   </si>
   <si>
-    <t>Content-Type:'text/plain; charset=utf-8'</t>
-  </si>
-  <si>
     <t>post</t>
   </si>
   <si>
     <t>get</t>
   </si>
   <si>
-    <t>http_get_test_02</t>
-  </si>
-  <si>
     <t>k1=v1&amp;k2=v2</t>
   </si>
   <si>
@@ -79,6 +64,36 @@
   </si>
   <si>
     <t>http://127.0.0.1:17891/index</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>smoke,module01,p1</t>
+  </si>
+  <si>
+    <t>RetCode</t>
+  </si>
+  <si>
+    <t>test_index_get_01</t>
+  </si>
+  <si>
+    <t>test_index_post_02</t>
+  </si>
+  <si>
+    <t>module01,p1</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>Content-Type:'text/plain; charset=utf-8',</t>
+  </si>
+  <si>
+    <t>Content-Type:'text/json; charset=utf-8',</t>
   </si>
 </sst>
 </file>
@@ -152,11 +167,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,23 +488,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E798D7C-3FAD-754F-9877-91756B700D0C}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-    <col min="5" max="5" width="35.1640625" customWidth="1"/>
-    <col min="6" max="6" width="44.6640625" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -496,77 +515,86 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1">
+        <v>200</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>9</v>
+      <c r="H3" s="1">
+        <v>200</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1">
-        <v>200</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1">
-        <v>200</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -575,11 +603,12 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{EC47FDFA-BB4B-4C4E-9638-E51829180CCB}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{F4D51686-6BC4-144F-B552-4DC7D886A320}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{EC47FDFA-BB4B-4C4E-9638-E51829180CCB}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{F4D51686-6BC4-144F-B552-4DC7D886A320}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix, and add api test cases.
</commit_message>
<xml_diff>
--- a/apitest/TestCases.xlsx
+++ b/apitest/TestCases.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengjin/Workspaces/zj_py3_project/apitest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BAEA5FC3-32B5-894E-BC36-33B32BB8E1A3}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46BE20DE-16C1-1B4F-9743-AC413C6C8093}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{C6BC2A70-CB81-DB40-9C8F-527C04FB6517}"/>
   </bookViews>
   <sheets>
     <sheet name="Module01" sheetId="1" r:id="rId1"/>
+    <sheet name="Module02" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="42">
   <si>
     <t>CaseId</t>
   </si>
@@ -57,9 +58,6 @@
     <t>get</t>
   </si>
   <si>
-    <t>k1=v1&amp;k2=v2</t>
-  </si>
-  <si>
     <t>Url</t>
   </si>
   <si>
@@ -78,25 +76,82 @@
     <t>test_index_get_01</t>
   </si>
   <si>
-    <t>test_index_post_02</t>
-  </si>
-  <si>
     <t>module01,p1</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>Content-Type:'text/plain; charset=utf-8',</t>
-  </si>
-  <si>
-    <t>Content-Type:'text/json; charset=utf-8',</t>
-  </si>
-  <si>
     <t>200</t>
+  </si>
+  <si>
+    <t>test_index_post_01</t>
+  </si>
+  <si>
+    <t>test_index_get_02</t>
+  </si>
+  <si>
+    <t>Content-Type:'text/plain; charset=utf-8'</t>
+  </si>
+  <si>
+    <t>Content-Type:'text/json; charset=utf-8'</t>
+  </si>
+  <si>
+    <t>isFile=true</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>./test.file</t>
+  </si>
+  <si>
+    <t>test_error_get_01</t>
+  </si>
+  <si>
+    <t>test_error_get_02</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:17891/error</t>
+  </si>
+  <si>
+    <t>retCode=206</t>
+  </si>
+  <si>
+    <t>retCode=200</t>
+  </si>
+  <si>
+    <t>retCode=400</t>
+  </si>
+  <si>
+    <t>206</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>test_error_get_03</t>
+  </si>
+  <si>
+    <t>b001</t>
+  </si>
+  <si>
+    <t>b002</t>
+  </si>
+  <si>
+    <t>b003</t>
+  </si>
+  <si>
+    <t>a001</t>
+  </si>
+  <si>
+    <t>a002</t>
+  </si>
+  <si>
+    <t>a003</t>
+  </si>
+  <si>
+    <t>isFile=false</t>
+  </si>
+  <si>
+    <t>Query</t>
   </si>
 </sst>
 </file>
@@ -491,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E798D7C-3FAD-754F-9877-91756B700D0C}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,12 +560,14 @@
     <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="25.5" customWidth="1"/>
     <col min="6" max="6" width="35.1640625" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" customWidth="1"/>
-    <col min="9" max="9" width="28" customWidth="1"/>
+    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -518,100 +575,311 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{EC47FDFA-BB4B-4C4E-9638-E51829180CCB}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{F4D51686-6BC4-144F-B552-4DC7D886A320}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{F4D51686-6BC4-144F-B552-4DC7D886A320}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{20259987-E2A2-9A49-8AA6-5292C1542AF2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6A30E5-BD00-E34B-A8FA-2D2682BE6DFD}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
+    <col min="6" max="6" width="35.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="28.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D5C663EB-BE5E-3143-9AC2-D4B1B61D6297}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{35A10555-E3C0-5A49-87E4-834F45E8574A}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{2BB026CD-3AAE-BF4D-A9C8-9561FCC3BC66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Fix, and add base test.
</commit_message>
<xml_diff>
--- a/apitest/TestCases.xlsx
+++ b/apitest/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengjin/Workspaces/zj_py3_project/apitest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{46BE20DE-16C1-1B4F-9743-AC413C6C8093}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{49F5FD9C-200A-4240-9A95-FDF2D1B883D5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15940" xr2:uid="{C6BC2A70-CB81-DB40-9C8F-527C04FB6517}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>{"email": "123456@163.com", "password": "123456"}</t>
   </si>
   <si>
-    <t>ExpectedMsg</t>
-  </si>
-  <si>
     <t>{"results": "ok"}</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>Query</t>
+  </si>
+  <si>
+    <t>RetMsg</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,120 +575,120 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -722,7 +722,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -748,116 +748,116 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>

</xml_diff>